<commit_message>
Updated experimental data and plots
Testing a co-dependency of Bg and Bth for the experimental data.
</commit_message>
<xml_diff>
--- a/Data/All Data.xlsx
+++ b/Data/All Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Jacobs\Documents\Projects\Dobrynin_Solution_Theory\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0242D98-55A5-441C-B482-658D02172319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF83CD95-BDA7-4A48-A95D-B12765C9B41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="122">
   <si>
     <t>cl^3</t>
   </si>
@@ -399,6 +399,9 @@
   <si>
     <t>Pe</t>
   </si>
+  <si>
+    <t>Bth(Bg)</t>
+  </si>
 </sst>
 </file>
 
@@ -11490,13 +11493,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86598AE-2DF5-4463-A7BF-B43F361AE836}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11508,7 +11511,7 @@
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -11542,8 +11545,11 @@
       <c r="L1" t="s">
         <v>120</v>
       </c>
+      <c r="M1" t="s">
+        <v>121</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11577,8 +11583,12 @@
       <c r="L2">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M2">
+        <f>0.38/0.7*J2+0.05</f>
+        <v>0.24108571428571429</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11612,8 +11622,12 @@
       <c r="L3">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M58" si="0">0.38/0.7*J3+0.05</f>
+        <v>0.24162857142857147</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11647,8 +11661,12 @@
       <c r="L4">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.24217142857142859</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11682,8 +11700,12 @@
       <c r="L5">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.25031428571428577</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11714,8 +11736,12 @@
       <c r="L6">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.26117142857142861</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11746,8 +11772,12 @@
       <c r="L7">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.27311428571428575</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11778,8 +11808,12 @@
       <c r="L8">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.2861428571428572</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11810,8 +11844,12 @@
       <c r="L9">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0.29428571428571432</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11842,8 +11880,12 @@
       <c r="L10">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0.29971428571428577</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11871,8 +11913,12 @@
       <c r="L11">
         <v>11.3</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0.4245714285714286</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11903,8 +11949,12 @@
       <c r="L12">
         <v>11.3</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11935,8 +11985,12 @@
       <c r="L13">
         <v>11.3</v>
       </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0.38657142857142862</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11967,8 +12021,12 @@
       <c r="L14">
         <v>11.3</v>
       </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.36485714285714288</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11999,8 +12057,12 @@
       <c r="L15">
         <v>11.3</v>
       </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>0.34857142857142864</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -12031,8 +12093,12 @@
       <c r="L16">
         <v>11.3</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.34314285714285719</v>
+      </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12063,8 +12129,12 @@
       <c r="L17">
         <v>11.3</v>
       </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>0.34314285714285719</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12089,11 +12159,18 @@
       <c r="J18">
         <v>0.47</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
       <c r="L18">
         <v>18</v>
       </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>0.30514285714285716</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -12118,11 +12195,18 @@
       <c r="J19">
         <v>0.4</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
       <c r="L19">
         <v>18</v>
       </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.26714285714285718</v>
+      </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -12150,8 +12234,12 @@
       <c r="L20">
         <v>7.2</v>
       </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0.65800000000000014</v>
+      </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12173,11 +12261,18 @@
       <c r="J21">
         <v>0.61</v>
       </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
       <c r="L21">
         <v>6.3</v>
       </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>0.38114285714285717</v>
+      </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -12205,8 +12300,12 @@
       <c r="L22">
         <v>4.4000000000000004</v>
       </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.45171428571428573</v>
+      </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -12234,8 +12333,12 @@
       <c r="L23">
         <v>4.4000000000000004</v>
       </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>0.45171428571428573</v>
+      </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -12263,8 +12366,12 @@
       <c r="L24">
         <v>12.6</v>
       </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>0.38657142857142862</v>
+      </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -12292,8 +12399,12 @@
       <c r="L25">
         <v>8.1</v>
       </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>0.44085714285714289</v>
+      </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12324,8 +12435,12 @@
       <c r="L26">
         <v>9.5</v>
       </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>0.31057142857142861</v>
+      </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12359,8 +12474,12 @@
       <c r="L27">
         <v>11.4</v>
       </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -12394,8 +12513,12 @@
       <c r="L28">
         <v>11.4</v>
       </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>0.26171428571428573</v>
+      </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -12429,8 +12552,12 @@
       <c r="L29">
         <v>18</v>
       </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>0.28342857142857147</v>
+      </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -12455,11 +12582,18 @@
       <c r="J30">
         <v>0.39</v>
       </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
       <c r="L30">
         <v>18</v>
       </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>0.26171428571428573</v>
+      </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -12493,8 +12627,12 @@
       <c r="L31">
         <v>18</v>
       </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>0.32142857142857145</v>
+      </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -12513,14 +12651,21 @@
       <c r="G32">
         <v>0</v>
       </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
       <c r="K32">
         <v>0.27</v>
       </c>
       <c r="L32">
         <v>6.5</v>
       </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -12548,8 +12693,12 @@
       <c r="L33">
         <v>3.3</v>
       </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -12577,8 +12726,12 @@
       <c r="L34">
         <v>7.2</v>
       </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -12606,8 +12759,12 @@
       <c r="L35">
         <v>5.8</v>
       </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -12635,8 +12792,12 @@
       <c r="L36">
         <v>7.6</v>
       </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>0.32142857142857145</v>
+      </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -12655,14 +12816,21 @@
       <c r="G37">
         <v>298</v>
       </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
       <c r="K37">
         <v>0.24</v>
       </c>
       <c r="L37">
         <v>7.2</v>
       </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -12693,8 +12861,12 @@
       <c r="L38">
         <v>12.7</v>
       </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>0.29428571428571432</v>
+      </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -12725,8 +12897,12 @@
       <c r="L39">
         <v>12.7</v>
       </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>0.28342857142857147</v>
+      </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -12751,11 +12927,18 @@
       <c r="J40">
         <v>0.61</v>
       </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
       <c r="L40">
         <v>3.7</v>
       </c>
+      <c r="M40">
+        <f t="shared" si="0"/>
+        <v>0.38114285714285717</v>
+      </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -12780,11 +12963,18 @@
       <c r="J41">
         <v>0.6</v>
       </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
       <c r="L41">
         <v>3.2</v>
       </c>
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>0.37571428571428572</v>
+      </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -12809,11 +12999,18 @@
       <c r="J42">
         <v>0.99</v>
       </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
       <c r="L42">
         <v>3.2</v>
       </c>
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>0.58742857142857152</v>
+      </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -12838,11 +13035,18 @@
       <c r="J43">
         <v>0.54</v>
       </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
       <c r="L43">
         <v>3.2</v>
       </c>
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>0.34314285714285719</v>
+      </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -12867,11 +13071,18 @@
       <c r="J44">
         <v>0.63</v>
       </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
       <c r="L44">
         <v>3.2</v>
       </c>
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -12902,8 +13113,12 @@
       <c r="L45">
         <v>9.6</v>
       </c>
+      <c r="M45">
+        <f t="shared" si="0"/>
+        <v>0.26714285714285718</v>
+      </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -12928,11 +13143,18 @@
       <c r="J46">
         <v>0.64</v>
       </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
       <c r="L46">
         <v>3.6</v>
       </c>
+      <c r="M46">
+        <f t="shared" si="0"/>
+        <v>0.39742857142857146</v>
+      </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -12957,11 +13179,18 @@
       <c r="J47">
         <v>0.43</v>
       </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
       <c r="L47">
         <v>3</v>
       </c>
+      <c r="M47">
+        <f t="shared" si="0"/>
+        <v>0.28342857142857147</v>
+      </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -12986,11 +13215,18 @@
       <c r="J48">
         <v>0.43</v>
       </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
       <c r="L48">
         <v>3.4</v>
       </c>
+      <c r="M48">
+        <f t="shared" si="0"/>
+        <v>0.28342857142857147</v>
+      </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -13021,8 +13257,12 @@
       <c r="L49">
         <v>10.8</v>
       </c>
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -13044,11 +13284,18 @@
       <c r="J50">
         <v>0.5</v>
       </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
       <c r="L50">
         <v>2.7</v>
       </c>
+      <c r="M50">
+        <f t="shared" si="0"/>
+        <v>0.32142857142857145</v>
+      </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -13070,11 +13317,18 @@
       <c r="J51">
         <v>0.49</v>
       </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
       <c r="L51">
         <v>2.9</v>
       </c>
+      <c r="M51">
+        <f t="shared" si="0"/>
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -13096,11 +13350,18 @@
       <c r="J52">
         <v>0.51</v>
       </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
       <c r="L52">
         <v>3.4</v>
       </c>
+      <c r="M52">
+        <f t="shared" si="0"/>
+        <v>0.3268571428571429</v>
+      </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -13122,14 +13383,21 @@
       <c r="G53">
         <v>298</v>
       </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
       <c r="K53">
         <v>0.23</v>
       </c>
       <c r="L53">
         <v>9.6999999999999993</v>
       </c>
+      <c r="M53">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -13151,11 +13419,21 @@
       <c r="G54">
         <v>298</v>
       </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
       <c r="L54">
         <v>4.4000000000000004</v>
       </c>
+      <c r="M54">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13180,11 +13458,18 @@
       <c r="J55">
         <v>0.41</v>
       </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
       <c r="L55">
         <v>2.6</v>
       </c>
+      <c r="M55">
+        <f t="shared" si="0"/>
+        <v>0.27257142857142858</v>
+      </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13215,8 +13500,12 @@
       <c r="L56">
         <v>8.6999999999999993</v>
       </c>
+      <c r="M56">
+        <f t="shared" si="0"/>
+        <v>0.47342857142857148</v>
+      </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13247,8 +13536,12 @@
       <c r="L57">
         <v>8.3000000000000007</v>
       </c>
+      <c r="M57">
+        <f t="shared" si="0"/>
+        <v>0.45714285714285718</v>
+      </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -13270,8 +13563,15 @@
       <c r="J58">
         <v>0.46</v>
       </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
       <c r="L58">
         <v>3.4</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="0"/>
+        <v>0.29971428571428577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>